<commit_message>
Minor edit in Gantt Chart
</commit_message>
<xml_diff>
--- a/Gantt Chart 2.xlsx
+++ b/Gantt Chart 2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GU 2022/Yr 2 Tri 2/Software Technologies - 2810ICT/Project Management/2810ICT-7810ICT-2023-Assignment/Assignment Part A/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nasrinzahiri/Desktop/Assignment2/2810ICT-7810ICT-Assignment-Project-A-Project-Management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564328C4-B0EA-1146-BED9-D333FD4CBA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE287C6-0BC8-7A43-8128-9C874F9E9837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{CDE15F11-1B19-463B-9B8F-DCEEEB99003F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Task</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Sydney Airbnb Data Analysis Tool Project</t>
   </si>
 </sst>
 </file>
@@ -148,7 +151,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -156,28 +159,185 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -279,7 +439,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -298,7 +458,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$17</c:f>
+              <c:f>Sheet1!$B$3:$B$18</c:f>
               <c:strCache>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
@@ -354,7 +514,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$17</c:f>
+              <c:f>Sheet1!$D$3:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="16"/>
@@ -420,7 +580,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -441,7 +601,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$17</c:f>
+              <c:f>Sheet1!$B$3:$B$18</c:f>
               <c:strCache>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
@@ -497,7 +657,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$17</c:f>
+              <c:f>Sheet1!$C$3:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1297,13 +1457,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8466</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>371474</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>147638</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1629,10 +1789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832D897B-BFD5-4877-A234-B1F3A09042BD}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1646,359 +1806,371 @@
     <col min="8" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:9" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5">
-        <f>E2-D2</f>
-        <v>35</v>
-      </c>
-      <c r="D2" s="6">
-        <v>45159</v>
-      </c>
-      <c r="E2" s="6">
-        <v>45194</v>
-      </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="5">
-        <f t="shared" ref="C3:C16" si="0">E3-D3</f>
-        <v>14</v>
-      </c>
-      <c r="D3" s="6">
-        <v>45170</v>
-      </c>
-      <c r="E3" s="6">
-        <v>45184</v>
-      </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+      <c r="A3" s="15">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7">
+        <f>E3-D3</f>
+        <v>35</v>
+      </c>
+      <c r="D3" s="8">
+        <v>45159</v>
+      </c>
+      <c r="E3" s="16">
+        <v>45194</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
+      <c r="A4" s="15">
+        <v>2</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7">
+        <f t="shared" ref="C4:C17" si="0">E4-D4</f>
+        <v>14</v>
+      </c>
+      <c r="D4" s="8">
+        <v>45170</v>
+      </c>
+      <c r="E4" s="16">
+        <v>45184</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="15">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C5" s="7">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="D4" s="6">
-        <f t="shared" ref="D4" si="1">E3</f>
+      <c r="D5" s="8">
+        <f t="shared" ref="D5" si="1">E4</f>
         <v>45184</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E5" s="16">
         <v>45212</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="I4" s="1"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="I5" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="15">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C6" s="7">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D6" s="8">
         <v>45208</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E6" s="16">
         <v>45229</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
     </row>
-    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
+    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="15">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C7" s="7">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D7" s="8">
         <v>45219</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E7" s="16">
         <v>45240</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
     </row>
-    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
+    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="15">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C8" s="7">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D8" s="8">
         <v>45239</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E8" s="16">
         <v>45260</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
     </row>
-    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
+    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="15">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C9" s="7">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D9" s="8">
         <v>45252</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E9" s="16">
         <v>45294</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
     </row>
-    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
+    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="15">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C10" s="7">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D10" s="8">
         <v>45262</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E10" s="16">
         <v>45297</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
     </row>
-    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
+    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="15">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C11" s="7">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D11" s="8">
         <v>45278</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E11" s="16">
         <v>45306</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
     </row>
-    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
+    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="15">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C12" s="7">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D12" s="8">
         <v>45292</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E12" s="16">
         <v>45313</v>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
     </row>
-    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
+    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="15">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C13" s="7">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D13" s="8">
         <v>45311</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E13" s="16">
         <v>45353</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
     </row>
-    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="7">
+    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="15">
         <v>12</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B14" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C14" s="7">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D14" s="8">
         <v>45336</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E14" s="16">
         <v>45364</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="I13" s="2"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="I14" s="2"/>
     </row>
-    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="7">
+    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="15">
         <v>13</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C15" s="7">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D15" s="8">
         <v>45343</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E15" s="16">
         <v>45357</v>
       </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
     </row>
-    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="7">
+    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="15">
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B16" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C16" s="7">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D16" s="8">
         <v>45352</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E16" s="16">
         <v>45380</v>
       </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
     </row>
-    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="7">
+    <row r="17" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="15">
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B17" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C17" s="7">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D17" s="8">
         <v>45370</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E17" s="16">
         <v>45391</v>
       </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
     </row>
-    <row r="17" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="7">
+    <row r="18" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="17">
         <v>16</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B18" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C18" s="19">
         <v>39</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D18" s="20">
         <v>45352</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E18" s="21">
         <v>45391</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F23" s="8"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F24" s="8"/>
+      <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H25" t="s">
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <dataValidations count="1">
-    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D17 I4" xr:uid="{62E48654-2731-42DC-B611-EED9655AA64A}"/>
+    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D18 I5" xr:uid="{62E48654-2731-42DC-B611-EED9655AA64A}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>